<commit_message>
connected to sparse matrix, minor edit to traindata
</commit_message>
<xml_diff>
--- a/Data_Ingestion/CDS_SPARSE_ENR.xlsx
+++ b/Data_Ingestion/CDS_SPARSE_ENR.xlsx
@@ -1,60 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimj16\Documents\497\rhit_IRPA_2023\Data_Ingestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bowending/Documents/rhit_IRPA_2023/Data_Ingestion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC85216-4646-49B9-8956-39BA974EA81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA14872-D0CE-E34E-B963-6A5ED543BBFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7092" yWindow="2916" windowWidth="14808" windowHeight="10116" activeTab="1" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
     <sheet name="Enrollment_by_Race" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
-  <si>
-    <t>undergrad</t>
-  </si>
-  <si>
-    <t>grad</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>full-time</t>
   </si>
   <si>
     <t>part-time</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>female</t>
   </si>
   <si>
     <t>degree-seeking</t>
@@ -109,6 +86,21 @@
   </si>
   <si>
     <t>two-or-more</t>
+  </si>
+  <si>
+    <t>graduate</t>
+  </si>
+  <si>
+    <t>undergraduate</t>
+  </si>
+  <si>
+    <t>men</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -462,60 +454,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224585FE-606B-4F40-9ACE-2F85812D2681}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>387</v>
       </c>
@@ -565,7 +560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>143</v>
       </c>
@@ -615,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -665,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -715,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>9</v>
       </c>
@@ -765,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -815,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -865,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0</v>
       </c>
@@ -915,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1082</v>
       </c>
@@ -965,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>329</v>
       </c>
@@ -1015,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>15</v>
       </c>
@@ -1065,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1115,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1478</v>
       </c>
@@ -1165,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>474</v>
       </c>
@@ -1215,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1265,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1315,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1365,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1415,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1465,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1515,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1478</v>
       </c>
@@ -1565,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>474</v>
       </c>
@@ -1615,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>18</v>
       </c>
@@ -1665,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1715,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1765,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1815,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1865,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1915,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1965,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2015,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5</v>
       </c>
@@ -2065,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0</v>
       </c>
@@ -2115,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0</v>
       </c>
@@ -2165,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0</v>
       </c>
@@ -2215,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
@@ -2265,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2315,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>9</v>
       </c>
@@ -2365,7 +2360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2415,7 +2410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>7</v>
       </c>
@@ -2465,7 +2460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2524,45 +2519,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EB211C-713F-433C-AADD-E85D0317D8A2}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>36</v>
       </c>
@@ -2597,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>226</v>
       </c>
@@ -2632,7 +2627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>34</v>
       </c>
@@ -2667,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>104</v>
       </c>
@@ -2702,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>31</v>
       </c>
@@ -2737,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>93</v>
       </c>
@@ -2772,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>356</v>
       </c>
@@ -2807,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1295</v>
       </c>
@@ -2842,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2877,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -2912,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>36</v>
       </c>
@@ -2947,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>127</v>
       </c>
@@ -2982,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3017,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3052,7 +3047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>31</v>
       </c>
@@ -3087,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>99</v>
       </c>
@@ -3122,7 +3117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6</v>
       </c>
@@ -3157,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>22</v>
       </c>
@@ -3192,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>531</v>
       </c>
@@ -3227,7 +3222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1969</v>
       </c>

</xml_diff>

<commit_message>
fixed bug with SparseMatrixKnowledgeBase adding up total and throwing error
</commit_message>
<xml_diff>
--- a/Data_Ingestion/CDS_SPARSE_ENR.xlsx
+++ b/Data_Ingestion/CDS_SPARSE_ENR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bowending/Documents/rhit_IRPA_2023/Data_Ingestion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\Data_Ingestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA14872-D0CE-E34E-B963-6A5ED543BBFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF999F7C-7C96-40B9-B9D6-E68ED4B4DFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
@@ -455,12 +455,15 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -510,7 +513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>387</v>
       </c>
@@ -560,7 +563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>143</v>
       </c>
@@ -610,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -660,7 +663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -710,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -760,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -810,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -860,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -910,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1082</v>
       </c>
@@ -960,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>329</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>15</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1110,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1478</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>474</v>
       </c>
@@ -1210,7 +1213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1410,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1478</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>474</v>
       </c>
@@ -1610,7 +1613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>18</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1810,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1860,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1910,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1960,7 +1963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2010,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>5</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0</v>
       </c>
@@ -2210,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2</v>
       </c>
@@ -2260,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2310,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>9</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2410,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>7</v>
       </c>
@@ -2460,7 +2463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2523,9 +2526,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>15</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>36</v>
       </c>
@@ -2592,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>226</v>
       </c>
@@ -2627,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>34</v>
       </c>
@@ -2662,7 +2665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>31</v>
       </c>
@@ -2732,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>93</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>356</v>
       </c>
@@ -2802,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1295</v>
       </c>
@@ -2837,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2872,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>36</v>
       </c>
@@ -2942,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>127</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3012,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3047,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>31</v>
       </c>
@@ -3082,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>99</v>
       </c>
@@ -3117,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6</v>
       </c>
@@ -3152,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>22</v>
       </c>
@@ -3187,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>531</v>
       </c>
@@ -3222,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1969</v>
       </c>

</xml_diff>

<commit_message>
added new columns to sparse matrix
</commit_message>
<xml_diff>
--- a/Data_Ingestion/CDS_SPARSE_ENR.xlsx
+++ b/Data_Ingestion/CDS_SPARSE_ENR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\Data_Ingestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimj16\Documents\497\rhit_IRPA_2023\Data_Ingestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF999F7C-7C96-40B9-B9D6-E68ED4B4DFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7487AE8-44A1-4963-84F0-35E55D7AD763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
+    <workbookView xWindow="15504" yWindow="1284" windowWidth="14808" windowHeight="10116" activeTab="1" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>full-time</t>
   </si>
@@ -454,14 +454,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224585FE-606B-4F40-9ACE-2F85812D2681}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="8.77734375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2520,15 +2517,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EB211C-713F-433C-AADD-E85D0317D8A2}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>15</v>
       </c>
@@ -2559,8 +2556,26 @@
       <c r="K1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>36</v>
       </c>
@@ -2594,8 +2609,26 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>226</v>
       </c>
@@ -2629,8 +2662,26 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>34</v>
       </c>
@@ -2664,8 +2715,26 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
@@ -2699,8 +2768,26 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>31</v>
       </c>
@@ -2734,8 +2821,26 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>93</v>
       </c>
@@ -2769,8 +2874,26 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>356</v>
       </c>
@@ -2804,8 +2927,26 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1295</v>
       </c>
@@ -2839,8 +2980,26 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2874,8 +3033,26 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -2909,8 +3086,26 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>36</v>
       </c>
@@ -2944,8 +3139,26 @@
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>127</v>
       </c>
@@ -2979,8 +3192,26 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3014,8 +3245,26 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3049,8 +3298,26 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>31</v>
       </c>
@@ -3084,8 +3351,26 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>99</v>
       </c>
@@ -3119,8 +3404,26 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6</v>
       </c>
@@ -3154,8 +3457,26 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>22</v>
       </c>
@@ -3189,8 +3510,26 @@
       <c r="K19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>531</v>
       </c>
@@ -3224,8 +3563,26 @@
       <c r="K20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1969</v>
       </c>
@@ -3257,6 +3614,24 @@
         <v>0</v>
       </c>
       <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added test cases and implement the search algorithm to consider multiple matrix for one section
</commit_message>
<xml_diff>
--- a/Data_Ingestion/CDS_SPARSE_ENR.xlsx
+++ b/Data_Ingestion/CDS_SPARSE_ENR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\Data_Ingestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF999F7C-7C96-40B9-B9D6-E68ED4B4DFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8A2E9E-D252-4E5C-AFA6-0C802B200C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>full-time</t>
   </si>
@@ -454,13 +454,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224585FE-606B-4F40-9ACE-2F85812D2681}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -2215,7 +2215,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -2265,7 +2265,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -2522,13 +2522,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EB211C-713F-433C-AADD-E85D0317D8A2}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
       <c r="B1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Added test for sparseMatrixKnowledgeBase, changed search function to take in ShouldAddRowStrategy, and to determine which matrix to use. Implemented ChooseFromOptionAddRowStrategy to handle enrollment by race
</commit_message>
<xml_diff>
--- a/Data_Ingestion/CDS_SPARSE_ENR.xlsx
+++ b/Data_Ingestion/CDS_SPARSE_ENR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\Data_Ingestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8A2E9E-D252-4E5C-AFA6-0C802B200C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350795E0-7352-4B04-BFAB-788398A5B683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>full-time</t>
   </si>
@@ -454,14 +454,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224585FE-606B-4F40-9ACE-2F85812D2681}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2520,13 +2517,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EB211C-713F-433C-AADD-E85D0317D8A2}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+    <col min="14" max="14" width="14.21875" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" customWidth="1"/>
+    <col min="18" max="18" width="10.109375" customWidth="1"/>
+    <col min="19" max="19" width="13.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2560,8 +2574,26 @@
       <c r="K1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>36</v>
       </c>
@@ -2595,8 +2627,26 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>226</v>
       </c>
@@ -2630,8 +2680,26 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>34</v>
       </c>
@@ -2665,8 +2733,26 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
@@ -2700,8 +2786,26 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>31</v>
       </c>
@@ -2735,8 +2839,26 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>93</v>
       </c>
@@ -2770,8 +2892,26 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>356</v>
       </c>
@@ -2805,8 +2945,26 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1295</v>
       </c>
@@ -2840,8 +2998,26 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2875,8 +3051,26 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -2910,8 +3104,26 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>36</v>
       </c>
@@ -2945,8 +3157,26 @@
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>127</v>
       </c>
@@ -2980,8 +3210,26 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3015,8 +3263,26 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3050,8 +3316,26 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>31</v>
       </c>
@@ -3085,8 +3369,26 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>99</v>
       </c>
@@ -3120,8 +3422,26 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6</v>
       </c>
@@ -3155,8 +3475,26 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>22</v>
       </c>
@@ -3190,8 +3528,26 @@
       <c r="K19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>531</v>
       </c>
@@ -3225,8 +3581,26 @@
       <c r="K20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1969</v>
       </c>
@@ -3258,6 +3632,24 @@
         <v>0</v>
       </c>
       <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added more test case, query for two or more race should work now, added entity is_first_year and training examples. Changed search so it answers a question to the best of its ability.
</commit_message>
<xml_diff>
--- a/Data_Ingestion/CDS_SPARSE_ENR.xlsx
+++ b/Data_Ingestion/CDS_SPARSE_ENR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\Data_Ingestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350795E0-7352-4B04-BFAB-788398A5B683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421D18B9-3BB5-46FB-9348-8446F2A233A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
@@ -16,10 +16,21 @@
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
     <sheet name="Enrollment_by_Race" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -85,9 +96,6 @@
     <t>pacific-islander</t>
   </si>
   <si>
-    <t>two-or-more</t>
-  </si>
-  <si>
     <t>graduate</t>
   </si>
   <si>
@@ -101,6 +109,9 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>two or more races</t>
   </si>
 </sst>
 </file>
@@ -454,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224585FE-606B-4F40-9ACE-2F85812D2681}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -462,25 +473,25 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -2520,7 +2531,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2529,7 +2540,7 @@
     <col min="4" max="4" width="15.5546875" customWidth="1"/>
     <col min="5" max="5" width="14.21875" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" customWidth="1"/>
     <col min="13" max="13" width="18.44140625" customWidth="1"/>
     <col min="14" max="14" width="14.21875" customWidth="1"/>
@@ -2542,7 +2553,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -2566,7 +2577,7 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
         <v>12</v>

</xml_diff>